<commit_message>
added optimization of style so common items are boiled up from cell to row to table level styles.
</commit_message>
<xml_diff>
--- a/ExcelToWiki/example/test.xlsx
+++ b/ExcelToWiki/example/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Test Bold</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>row width 2"</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -111,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +157,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -155,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -171,6 +192,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -517,67 +539,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="8" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="7"/>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="7"/>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="C7" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="7"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="A6:B7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added a hyper link example
</commit_message>
<xml_diff>
--- a/ExcelToWiki/example/test.xlsx
+++ b/ExcelToWiki/example/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Test Bold</t>
   </si>
@@ -70,13 +70,16 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>http://yahoo.com Yahoo!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,6 +126,14 @@
       <sz val="12"/>
       <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -173,16 +184,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -192,9 +205,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,7 +541,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -539,19 +553,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -578,36 +592,39 @@
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="8"/>
       <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="7"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:5">
+      <c r="A8" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
@@ -618,6 +635,9 @@
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="A6:B7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" display="http://yahoo.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
added multiline element in excel file test bugfixed several mistakes in style processing
</commit_message>
<xml_diff>
--- a/ExcelToWiki/example/test.xlsx
+++ b/ExcelToWiki/example/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32700" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Test Bold</t>
   </si>
@@ -73,13 +73,20 @@
   </si>
   <si>
     <t>http://yahoo.com Yahoo!</t>
+  </si>
+  <si>
+    <t>* test1
+* test2</t>
+  </si>
+  <si>
+    <t>Test italics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,6 +141,13 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -188,7 +202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -196,6 +210,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -205,7 +224,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -538,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -579,6 +597,9 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
@@ -592,41 +613,46 @@
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="8"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="11"/>
       <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>